<commit_message>
nuevo archivo update registro e idea aplicacion final
</commit_message>
<xml_diff>
--- a/Project1/CalendarExport.xlsx
+++ b/Project1/CalendarExport.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CLPU\Desarrollo\Rep-Git-1\Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trabajo personal\Tesis_2024\development\Rep-Git-1\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C558EF60-648C-4E78-9133-2A84A4E8ABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159" uniqueCount="127">
   <si>
     <t>Galán Prado, Fabio</t>
   </si>
@@ -286,13 +288,127 @@
   </si>
   <si>
     <t>lunes, viernes</t>
+  </si>
+  <si>
+    <t>Descripción base de datos.</t>
+  </si>
+  <si>
+    <t>CALENDARIO</t>
+  </si>
+  <si>
+    <t>Dia_year</t>
+  </si>
+  <si>
+    <t>Dia_semana</t>
+  </si>
+  <si>
+    <t>Lectivo</t>
+  </si>
+  <si>
+    <t>Modo_trabajo</t>
+  </si>
+  <si>
+    <t>Personas_T1</t>
+  </si>
+  <si>
+    <t>Personas_T2</t>
+  </si>
+  <si>
+    <t>Personas_T3</t>
+  </si>
+  <si>
+    <t>Personas_vacaciones</t>
+  </si>
+  <si>
+    <t>Personas_baja</t>
+  </si>
+  <si>
+    <t>Personas_medico</t>
+  </si>
+  <si>
+    <t>Personas_teletrabajo</t>
+  </si>
+  <si>
+    <t>Personas_teletrabajo_tarde</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Tipo_horario</t>
+  </si>
+  <si>
+    <t>Conciliacion</t>
+  </si>
+  <si>
+    <t>D_teletrabajo</t>
+  </si>
+  <si>
+    <t>ND_campaign</t>
+  </si>
+  <si>
+    <t>Tipo_T</t>
+  </si>
+  <si>
+    <t>T1_H1</t>
+  </si>
+  <si>
+    <t>RECUENTO</t>
+  </si>
+  <si>
+    <t>MNT_M</t>
+  </si>
+  <si>
+    <t>DEV_MNT_M</t>
+  </si>
+  <si>
+    <t>MNT_T</t>
+  </si>
+  <si>
+    <t>DEV_MNT_T</t>
+  </si>
+  <si>
+    <t>CI_M</t>
+  </si>
+  <si>
+    <t>DEV_CI_M</t>
+  </si>
+  <si>
+    <t>CI_T</t>
+  </si>
+  <si>
+    <t>DEV_CI_T</t>
+  </si>
+  <si>
+    <t>CE_M</t>
+  </si>
+  <si>
+    <t>DEV_CE_M</t>
+  </si>
+  <si>
+    <t>CE_T</t>
+  </si>
+  <si>
+    <t>DEV_CE_T</t>
+  </si>
+  <si>
+    <t>TOTAL_M</t>
+  </si>
+  <si>
+    <t>DEV_TOTAL_M</t>
+  </si>
+  <si>
+    <t>TOTAL_T</t>
+  </si>
+  <si>
+    <t>DEV_TOTAL_T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,8 +458,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +594,11 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -743,13 +871,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -766,8 +895,8 @@
     <xf numFmtId="14" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -820,13 +949,13 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="19" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="20" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
@@ -839,9 +968,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="12" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="3" builtinId="10"/>
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
@@ -1143,28 +1274,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="32" width="3.7109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="2.42578125" customWidth="1"/>
-    <col min="37" max="37" width="16.85546875" customWidth="1"/>
-    <col min="38" max="38" width="13.140625" customWidth="1"/>
-    <col min="40" max="40" width="11.7109375" customWidth="1"/>
-    <col min="41" max="41" width="12.5703125" customWidth="1"/>
+    <col min="2" max="32" width="3.6640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="2.44140625" customWidth="1"/>
+    <col min="37" max="37" width="16.88671875" customWidth="1"/>
+    <col min="38" max="38" width="13.109375" customWidth="1"/>
+    <col min="40" max="40" width="11.6640625" customWidth="1"/>
+    <col min="41" max="41" width="12.5546875" customWidth="1"/>
     <col min="42" max="42" width="18" customWidth="1"/>
     <col min="48" max="48" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:48" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:48" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
@@ -1262,7 +1393,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1506,7 @@
       <c r="AP3" s="64"/>
       <c r="AQ3" s="64"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1500,7 +1631,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1748,7 @@
       <c r="AP5" s="30"/>
       <c r="AQ5" s="30"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -1738,7 +1869,7 @@
       <c r="AP6" s="30"/>
       <c r="AQ6" s="30"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
@@ -1859,7 +1990,7 @@
       <c r="AP7" s="30"/>
       <c r="AQ7" s="30"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
@@ -1957,7 +2088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
@@ -2055,7 +2186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -2153,8 +2284,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:48" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:48" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -2243,7 +2374,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2505,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>6</v>
       </c>
@@ -2501,7 +2632,7 @@
       </c>
       <c r="AV14" s="62"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>7</v>
       </c>
@@ -2628,7 +2759,7 @@
       </c>
       <c r="AV15" s="62"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
@@ -2755,7 +2886,7 @@
       </c>
       <c r="AV16" s="62"/>
     </row>
-    <row r="17" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>9</v>
       </c>
@@ -2884,7 +3015,7 @@
       </c>
       <c r="AV17" s="62"/>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>10</v>
       </c>
@@ -3013,7 +3144,7 @@
       </c>
       <c r="AV18" s="62"/>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>11</v>
       </c>
@@ -3140,7 +3271,7 @@
       </c>
       <c r="AV19" s="62"/>
     </row>
-    <row r="20" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
@@ -3259,7 +3390,7 @@
       </c>
       <c r="AV20" s="62"/>
     </row>
-    <row r="21" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AK21" s="30" t="s">
         <v>61</v>
       </c>
@@ -3291,7 +3422,7 @@
       </c>
       <c r="AV21" s="62"/>
     </row>
-    <row r="22" spans="1:48" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>17</v>
       </c>
@@ -3389,7 +3520,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -3487,7 +3618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>6</v>
       </c>
@@ -3585,7 +3716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
@@ -3683,7 +3814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
@@ -3781,7 +3912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>9</v>
       </c>
@@ -3879,7 +4010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>10</v>
       </c>
@@ -3977,7 +4108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>11</v>
       </c>
@@ -4075,7 +4206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>12</v>
       </c>
@@ -4173,8 +4304,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:48" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:48" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
@@ -4269,7 +4400,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>0</v>
       </c>
@@ -4364,7 +4495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>6</v>
       </c>
@@ -4459,7 +4590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>7</v>
       </c>
@@ -4554,7 +4685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -4649,7 +4780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>9</v>
       </c>
@@ -4744,7 +4875,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>10</v>
       </c>
@@ -4839,7 +4970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>11</v>
       </c>
@@ -4934,7 +5065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>12</v>
       </c>
@@ -5029,8 +5160,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:32" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>19</v>
       </c>
@@ -5128,7 +5259,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>0</v>
       </c>
@@ -5226,7 +5357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>6</v>
       </c>
@@ -5324,7 +5455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>7</v>
       </c>
@@ -5422,7 +5553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>8</v>
       </c>
@@ -5520,7 +5651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>9</v>
       </c>
@@ -5618,7 +5749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>10</v>
       </c>
@@ -5716,7 +5847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>11</v>
       </c>
@@ -5814,7 +5945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>12</v>
       </c>
@@ -5912,8 +6043,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:32" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>20</v>
       </c>
@@ -6008,7 +6139,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="53" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>0</v>
       </c>
@@ -6103,7 +6234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>6</v>
       </c>
@@ -6198,7 +6329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>7</v>
       </c>
@@ -6293,7 +6424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>8</v>
       </c>
@@ -6388,7 +6519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>9</v>
       </c>
@@ -6483,7 +6614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>10</v>
       </c>
@@ -6578,7 +6709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>11</v>
       </c>
@@ -6673,7 +6804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>12</v>
       </c>
@@ -6768,8 +6899,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="62" spans="1:32" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>21</v>
       </c>
@@ -6867,7 +6998,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="63" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>0</v>
       </c>
@@ -6965,7 +7096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>6</v>
       </c>
@@ -7063,7 +7194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>7</v>
       </c>
@@ -7161,7 +7292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>8</v>
       </c>
@@ -7259,7 +7390,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>9</v>
       </c>
@@ -7357,7 +7488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>10</v>
       </c>
@@ -7455,7 +7586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>11</v>
       </c>
@@ -7553,7 +7684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>12</v>
       </c>
@@ -7651,8 +7782,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:34" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:34" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>22</v>
       </c>
@@ -7752,7 +7883,7 @@
       <c r="AG72" s="1"/>
       <c r="AH72" s="1"/>
     </row>
-    <row r="73" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>0</v>
       </c>
@@ -7852,7 +7983,7 @@
       <c r="AG73" s="1"/>
       <c r="AH73" s="1"/>
     </row>
-    <row r="74" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>6</v>
       </c>
@@ -7952,7 +8083,7 @@
       <c r="AG74" s="1"/>
       <c r="AH74" s="1"/>
     </row>
-    <row r="75" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>7</v>
       </c>
@@ -8052,7 +8183,7 @@
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
     </row>
-    <row r="76" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>8</v>
       </c>
@@ -8152,7 +8283,7 @@
       <c r="AG76" s="1"/>
       <c r="AH76" s="1"/>
     </row>
-    <row r="77" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>9</v>
       </c>
@@ -8252,7 +8383,7 @@
       <c r="AG77" s="1"/>
       <c r="AH77" s="1"/>
     </row>
-    <row r="78" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>10</v>
       </c>
@@ -8352,7 +8483,7 @@
       <c r="AG78" s="1"/>
       <c r="AH78" s="1"/>
     </row>
-    <row r="79" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>11</v>
       </c>
@@ -8452,7 +8583,7 @@
       <c r="AG79" s="1"/>
       <c r="AH79" s="1"/>
     </row>
-    <row r="80" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11" t="s">
         <v>12</v>
       </c>
@@ -8552,11 +8683,11 @@
       <c r="AG80" s="1"/>
       <c r="AH80" s="1"/>
     </row>
-    <row r="81" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AG81" s="1"/>
       <c r="AH81" s="1"/>
     </row>
-    <row r="82" spans="1:34" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>23</v>
       </c>
@@ -8653,7 +8784,7 @@
       <c r="AG82" s="1"/>
       <c r="AH82" s="1"/>
     </row>
-    <row r="83" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>0</v>
       </c>
@@ -8750,7 +8881,7 @@
       <c r="AG83" s="1"/>
       <c r="AH83" s="1"/>
     </row>
-    <row r="84" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
         <v>6</v>
       </c>
@@ -8847,7 +8978,7 @@
       <c r="AG84" s="1"/>
       <c r="AH84" s="1"/>
     </row>
-    <row r="85" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="10" t="s">
         <v>7</v>
       </c>
@@ -8944,7 +9075,7 @@
       <c r="AG85" s="1"/>
       <c r="AH85" s="1"/>
     </row>
-    <row r="86" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="s">
         <v>8</v>
       </c>
@@ -9041,7 +9172,7 @@
       <c r="AG86" s="1"/>
       <c r="AH86" s="1"/>
     </row>
-    <row r="87" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="10" t="s">
         <v>9</v>
       </c>
@@ -9138,7 +9269,7 @@
       <c r="AG87" s="1"/>
       <c r="AH87" s="1"/>
     </row>
-    <row r="88" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="10" t="s">
         <v>10</v>
       </c>
@@ -9235,7 +9366,7 @@
       <c r="AG88" s="1"/>
       <c r="AH88" s="1"/>
     </row>
-    <row r="89" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="10" t="s">
         <v>11</v>
       </c>
@@ -9332,7 +9463,7 @@
       <c r="AG89" s="1"/>
       <c r="AH89" s="1"/>
     </row>
-    <row r="90" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="11" t="s">
         <v>12</v>
       </c>
@@ -9429,8 +9560,8 @@
       <c r="AG90" s="1"/>
       <c r="AH90" s="1"/>
     </row>
-    <row r="91" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="1:34" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="1:34" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
         <v>24</v>
       </c>
@@ -9528,7 +9659,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="s">
         <v>0</v>
       </c>
@@ -9626,7 +9757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="s">
         <v>6</v>
       </c>
@@ -9724,7 +9855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="s">
         <v>7</v>
       </c>
@@ -9822,7 +9953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>8</v>
       </c>
@@ -9920,7 +10051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>9</v>
       </c>
@@ -10018,7 +10149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
         <v>10</v>
       </c>
@@ -10116,7 +10247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>11</v>
       </c>
@@ -10214,7 +10345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="11" t="s">
         <v>12</v>
       </c>
@@ -10312,8 +10443,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="102" spans="1:32" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>25</v>
       </c>
@@ -10408,7 +10539,7 @@
         <v>45991</v>
       </c>
     </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A103" s="10" t="s">
         <v>0</v>
       </c>
@@ -10503,7 +10634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="s">
         <v>6</v>
       </c>
@@ -10598,7 +10729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="s">
         <v>7</v>
       </c>
@@ -10693,7 +10824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="s">
         <v>8</v>
       </c>
@@ -10788,7 +10919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>9</v>
       </c>
@@ -10883,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
         <v>10</v>
       </c>
@@ -10978,7 +11109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>11</v>
       </c>
@@ -11073,7 +11204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="11" t="s">
         <v>12</v>
       </c>
@@ -11168,8 +11299,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="112" spans="1:32" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="1:32" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
         <v>26</v>
       </c>
@@ -11267,7 +11398,7 @@
         <v>46022</v>
       </c>
     </row>
-    <row r="113" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="10" t="s">
         <v>0</v>
       </c>
@@ -11365,7 +11496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>6</v>
       </c>
@@ -11463,7 +11594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>7</v>
       </c>
@@ -11561,7 +11692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="10" t="s">
         <v>8</v>
       </c>
@@ -11659,7 +11790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
         <v>9</v>
       </c>
@@ -11757,7 +11888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="10" t="s">
         <v>10</v>
       </c>
@@ -11855,7 +11986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="s">
         <v>11</v>
       </c>
@@ -11953,7 +12084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="11" t="s">
         <v>12</v>
       </c>
@@ -12059,4 +12190,221 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165DA2ED-C87A-4C00-9B65-A2E12C85A25E}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17:J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D6" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="65" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D8" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D9" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D10" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D11" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D12" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D13" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D14" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D18" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="J19" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="J20" s="30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="J21" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="J22" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="J23" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>